<commit_message>
work on multi referential
</commit_message>
<xml_diff>
--- a/storage/app/repository/ISO27001-2022.fr.xlsx
+++ b/storage/app/repository/ISO27001-2022.fr.xlsx
@@ -2479,12 +2479,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2521,7 +2527,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2534,12 +2540,16 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2555,6 +2565,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF729FCF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -2565,14 +2635,17 @@
   </sheetPr>
   <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A96" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="16.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="30"/>
@@ -2619,13 +2692,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -2643,7 +2716,7 @@
       <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -2651,13 +2724,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -2675,7 +2748,7 @@
       <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -2683,13 +2756,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -2701,13 +2774,13 @@
       <c r="F4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -2715,13 +2788,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2736,13 +2809,13 @@
       <c r="G5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="6" t="s">
         <v>41</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -2750,13 +2823,13 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -2771,13 +2844,13 @@
       <c r="G6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>47</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="6" t="s">
         <v>49</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -2785,13 +2858,13 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2812,7 +2885,7 @@
       <c r="I7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="6" t="s">
         <v>57</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -2820,13 +2893,13 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -2841,13 +2914,13 @@
       <c r="G8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="6" t="s">
         <v>63</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="6" t="s">
         <v>65</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -2855,13 +2928,13 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -2876,27 +2949,27 @@
       <c r="G9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="6" t="s">
         <v>73</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -2911,13 +2984,13 @@
       <c r="G10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="6" t="s">
         <v>81</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -2925,13 +2998,13 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2946,13 +3019,13 @@
       <c r="G11" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="6" t="s">
         <v>87</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="6" t="s">
         <v>81</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -2960,13 +3033,13 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -2981,13 +3054,13 @@
       <c r="G12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="6" t="s">
         <v>94</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="6" t="s">
         <v>96</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -2995,13 +3068,13 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -3016,13 +3089,13 @@
       <c r="G13" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="6" t="s">
         <v>102</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -3030,13 +3103,13 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -3051,13 +3124,13 @@
       <c r="G14" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="6" t="s">
         <v>49</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -3065,13 +3138,13 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="A15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -3086,13 +3159,13 @@
       <c r="G15" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="6" t="s">
         <v>116</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="6" t="s">
         <v>118</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -3100,13 +3173,13 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -3121,13 +3194,13 @@
       <c r="G16" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="6" t="s">
         <v>124</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" s="6" t="s">
         <v>118</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -3135,13 +3208,13 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -3156,13 +3229,13 @@
       <c r="G17" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="6" t="s">
         <v>131</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="6" t="s">
         <v>118</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -3170,13 +3243,13 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -3191,27 +3264,27 @@
       <c r="G18" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="6" t="s">
         <v>138</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="6" t="s">
         <v>118</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="19" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -3226,13 +3299,13 @@
       <c r="G19" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="6" t="s">
         <v>145</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="6" t="s">
         <v>118</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -3240,13 +3313,13 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="A20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -3261,13 +3334,13 @@
       <c r="G20" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="6" t="s">
         <v>151</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="6" t="s">
         <v>118</v>
       </c>
       <c r="K20" s="2" t="s">
@@ -3275,13 +3348,13 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="A21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -3302,7 +3375,7 @@
       <c r="I21" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J21" s="6" t="s">
         <v>118</v>
       </c>
       <c r="K21" s="2" t="s">
@@ -3310,13 +3383,13 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -3331,13 +3404,13 @@
       <c r="G22" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="6" t="s">
         <v>163</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="J22" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K22" s="2" t="s">
@@ -3345,13 +3418,13 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="A23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -3366,13 +3439,13 @@
       <c r="G23" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="6" t="s">
         <v>171</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K23" s="2" t="s">
@@ -3380,13 +3453,13 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="A24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -3401,13 +3474,13 @@
       <c r="G24" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="6" t="s">
         <v>176</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K24" s="2" t="s">
@@ -3415,13 +3488,13 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="A25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -3436,13 +3509,13 @@
       <c r="G25" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="6" t="s">
         <v>181</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="J25" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K25" s="2" t="s">
@@ -3450,13 +3523,13 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="A26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -3471,13 +3544,13 @@
       <c r="G26" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="6" t="s">
         <v>188</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J26" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K26" s="2" t="s">
@@ -3485,13 +3558,13 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="A27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3506,13 +3579,13 @@
       <c r="G27" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="6" t="s">
         <v>195</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="J27" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K27" s="2" t="s">
@@ -3520,19 +3593,19 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="A28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="6" t="s">
         <v>199</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -3541,13 +3614,13 @@
       <c r="G28" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="J28" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K28" s="2" t="s">
@@ -3555,13 +3628,13 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="A29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -3576,13 +3649,13 @@
       <c r="G29" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="6" t="s">
         <v>209</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="J29" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K29" s="2" t="s">
@@ -3590,13 +3663,13 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="A30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -3611,13 +3684,13 @@
       <c r="G30" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="H30" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="I30" s="5" t="s">
+      <c r="I30" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="J30" s="6" t="s">
         <v>218</v>
       </c>
       <c r="K30" s="2" t="s">
@@ -3625,13 +3698,13 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="A31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -3646,13 +3719,13 @@
       <c r="G31" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H31" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="I31" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="J31" s="6" t="s">
         <v>218</v>
       </c>
       <c r="K31" s="2" t="s">
@@ -3660,13 +3733,13 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="A32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -3681,13 +3754,13 @@
       <c r="G32" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="H32" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="I32" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="J32" s="6" t="s">
         <v>233</v>
       </c>
       <c r="K32" s="2" t="s">
@@ -3695,13 +3768,13 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="A33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3716,13 +3789,13 @@
       <c r="G33" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="H33" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="I33" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="J33" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K33" s="2" t="s">
@@ -3730,13 +3803,13 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="A34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -3751,13 +3824,13 @@
       <c r="G34" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="H34" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="I34" s="5" t="s">
+      <c r="I34" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="J34" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K34" s="2" t="s">
@@ -3765,13 +3838,13 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="1" t="s">
+      <c r="A35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -3786,13 +3859,13 @@
       <c r="G35" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="H35" s="6" t="s">
         <v>253</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="J35" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K35" s="2" t="s">
@@ -3800,13 +3873,13 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="1" t="s">
+      <c r="A36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -3821,13 +3894,13 @@
       <c r="G36" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="H36" s="6" t="s">
         <v>260</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="J36" s="5" t="s">
+      <c r="J36" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K36" s="2" t="s">
@@ -3835,13 +3908,13 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="A37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -3856,13 +3929,13 @@
       <c r="G37" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H37" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="I37" s="5" t="s">
+      <c r="I37" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="J37" s="5" t="s">
+      <c r="J37" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K37" s="2" t="s">
@@ -3870,13 +3943,13 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="A38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -3891,27 +3964,27 @@
       <c r="G38" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="H38" s="6" t="s">
         <v>274</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="J38" s="5" t="s">
+      <c r="J38" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="1" t="s">
+    <row r="39" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -3926,13 +3999,13 @@
       <c r="G39" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="H39" s="6" t="s">
         <v>281</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="J39" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K39" s="2" t="s">
@@ -3940,13 +4013,13 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="A40" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -3961,13 +4034,13 @@
       <c r="G40" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="H40" s="6" t="s">
         <v>288</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="J40" s="5" t="s">
+      <c r="J40" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K40" s="2" t="s">
@@ -3975,13 +4048,13 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="A41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -3996,13 +4069,13 @@
       <c r="G41" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="H41" s="6" t="s">
         <v>295</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="J41" s="5" t="s">
+      <c r="J41" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K41" s="2" t="s">
@@ -4010,13 +4083,13 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="1" t="s">
+      <c r="A42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -4028,27 +4101,27 @@
       <c r="F42" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="H42" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="J42" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="K42" s="6" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="A43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="5" t="s">
         <v>306</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -4063,13 +4136,13 @@
       <c r="G43" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="H43" s="5" t="s">
+      <c r="H43" s="6" t="s">
         <v>311</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="J43" s="5" t="s">
+      <c r="J43" s="6" t="s">
         <v>313</v>
       </c>
       <c r="K43" s="2" t="s">
@@ -4077,13 +4150,13 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="A44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="5" t="s">
         <v>306</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -4098,13 +4171,13 @@
       <c r="G44" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="H44" s="6" t="s">
         <v>318</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="J44" s="6" t="s">
         <v>320</v>
       </c>
       <c r="K44" s="2" t="s">
@@ -4112,13 +4185,13 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="A45" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="5" t="s">
         <v>306</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -4133,13 +4206,13 @@
       <c r="G45" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="H45" s="5" t="s">
+      <c r="H45" s="6" t="s">
         <v>326</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="J45" s="5" t="s">
+      <c r="J45" s="6" t="s">
         <v>328</v>
       </c>
       <c r="K45" s="2" t="s">
@@ -4147,13 +4220,13 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="A46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="5" t="s">
         <v>306</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -4168,13 +4241,13 @@
       <c r="G46" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="H46" s="5" t="s">
+      <c r="H46" s="6" t="s">
         <v>334</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="J46" s="5" t="s">
+      <c r="J46" s="6" t="s">
         <v>336</v>
       </c>
       <c r="K46" s="2" t="s">
@@ -4182,13 +4255,13 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="A47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="5" t="s">
         <v>306</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -4203,13 +4276,13 @@
       <c r="G47" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="H47" s="5" t="s">
+      <c r="H47" s="6" t="s">
         <v>342</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="J47" s="5" t="s">
+      <c r="J47" s="6" t="s">
         <v>344</v>
       </c>
       <c r="K47" s="2" t="s">
@@ -4217,13 +4290,13 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B48" s="1" t="s">
+      <c r="A48" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="5" t="s">
         <v>306</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -4238,13 +4311,13 @@
       <c r="G48" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="H48" s="5" t="s">
+      <c r="H48" s="6" t="s">
         <v>350</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="J48" s="5" t="s">
+      <c r="J48" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K48" s="2" t="s">
@@ -4252,13 +4325,13 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="A49" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="5" t="s">
         <v>306</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -4273,13 +4346,13 @@
       <c r="G49" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="H49" s="5" t="s">
+      <c r="H49" s="6" t="s">
         <v>357</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="J49" s="5" t="s">
+      <c r="J49" s="6" t="s">
         <v>96</v>
       </c>
       <c r="K49" s="2" t="s">
@@ -4287,13 +4360,13 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="A50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="5" t="s">
         <v>306</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -4308,13 +4381,13 @@
       <c r="G50" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="H50" s="5" t="s">
+      <c r="H50" s="6" t="s">
         <v>364</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="J50" s="5" t="s">
+      <c r="J50" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K50" s="2" t="s">
@@ -4322,13 +4395,13 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B51" s="1" t="s">
+      <c r="A51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -4337,16 +4410,16 @@
       <c r="E51" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F51" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="H51" s="5" t="s">
+      <c r="H51" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="I51" s="5" t="s">
+      <c r="I51" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="J51" s="5" t="s">
+      <c r="J51" s="6" t="s">
         <v>19</v>
       </c>
       <c r="K51" s="2" t="s">
@@ -4354,13 +4427,13 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="A52" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -4375,13 +4448,13 @@
       <c r="G52" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="H52" s="6" t="s">
         <v>379</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="J52" s="5" t="s">
+      <c r="J52" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K52" s="2" t="s">
@@ -4389,13 +4462,13 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B53" s="1" t="s">
+      <c r="A53" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -4410,13 +4483,13 @@
       <c r="G53" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="H53" s="5" t="s">
+      <c r="H53" s="6" t="s">
         <v>386</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="J53" s="5" t="s">
+      <c r="J53" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K53" s="2" t="s">
@@ -4424,13 +4497,13 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B54" s="1" t="s">
+      <c r="A54" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -4445,13 +4518,13 @@
       <c r="G54" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="H54" s="6" t="s">
         <v>393</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="J54" s="5" t="s">
+      <c r="J54" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K54" s="2" t="s">
@@ -4459,13 +4532,13 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B55" s="1" t="s">
+      <c r="A55" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -4480,13 +4553,13 @@
       <c r="G55" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H55" s="6" t="s">
         <v>400</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="J55" s="5" t="s">
+      <c r="J55" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K55" s="2" t="s">
@@ -4494,13 +4567,13 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B56" s="1" t="s">
+      <c r="A56" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -4515,13 +4588,13 @@
       <c r="G56" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="H56" s="5" t="s">
+      <c r="H56" s="6" t="s">
         <v>406</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="J56" s="5" t="s">
+      <c r="J56" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K56" s="2" t="s">
@@ -4529,13 +4602,13 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B57" s="1" t="s">
+      <c r="A57" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -4550,13 +4623,13 @@
       <c r="G57" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="H57" s="5" t="s">
+      <c r="H57" s="6" t="s">
         <v>412</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="J57" s="5" t="s">
+      <c r="J57" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K57" s="2" t="s">
@@ -4564,13 +4637,13 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B58" s="1" t="s">
+      <c r="A58" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -4585,27 +4658,27 @@
       <c r="G58" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="H58" s="5" t="s">
+      <c r="H58" s="6" t="s">
         <v>419</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="J58" s="5" t="s">
+      <c r="J58" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="K58" s="5" t="s">
+      <c r="K58" s="6" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B59" s="1" t="s">
+      <c r="A59" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -4620,13 +4693,13 @@
       <c r="G59" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="H59" s="6" t="s">
         <v>425</v>
       </c>
-      <c r="I59" s="5" t="s">
+      <c r="I59" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="J59" s="5" t="s">
+      <c r="J59" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K59" s="2" t="s">
@@ -4634,13 +4707,13 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B60" s="1" t="s">
+      <c r="A60" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -4655,27 +4728,27 @@
       <c r="G60" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="H60" s="5" t="s">
+      <c r="H60" s="6" t="s">
         <v>431</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="J60" s="5" t="s">
+      <c r="J60" s="6" t="s">
         <v>433</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61" s="1" t="s">
+    <row r="61" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -4690,13 +4763,13 @@
       <c r="G61" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="H61" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="I61" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="J61" s="5" t="s">
+      <c r="J61" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K61" s="2" t="s">
@@ -4704,13 +4777,13 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="A62" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -4725,13 +4798,13 @@
       <c r="G62" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="H62" s="6" t="s">
         <v>445</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="J62" s="5" t="s">
+      <c r="J62" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K62" s="2" t="s">
@@ -4739,13 +4812,13 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B63" s="1" t="s">
+      <c r="A63" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -4760,13 +4833,13 @@
       <c r="G63" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H63" s="6" t="s">
         <v>452</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="J63" s="5" t="s">
+      <c r="J63" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K63" s="2" t="s">
@@ -4774,13 +4847,13 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B64" s="1" t="s">
+      <c r="A64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -4795,13 +4868,13 @@
       <c r="G64" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H64" s="6" t="s">
         <v>459</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="J64" s="5" t="s">
+      <c r="J64" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K64" s="2" t="s">
@@ -4809,13 +4882,13 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B65" s="1" t="s">
+      <c r="A65" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="5" t="s">
         <v>374</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -4830,13 +4903,13 @@
       <c r="G65" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H65" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="I65" s="5" t="s">
+      <c r="I65" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="J65" s="5" t="s">
+      <c r="J65" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K65" s="2" t="s">
@@ -4844,13 +4917,13 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B66" s="1" t="s">
+      <c r="A66" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -4862,13 +4935,13 @@
       <c r="F66" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H66" s="6" t="s">
         <v>472</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="J66" s="5" t="s">
+      <c r="J66" s="6" t="s">
         <v>19</v>
       </c>
       <c r="K66" s="2" t="s">
@@ -4876,13 +4949,13 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B67" s="1" t="s">
+      <c r="A67" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -4891,16 +4964,16 @@
       <c r="E67" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F67" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="H67" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="I67" s="5" t="s">
+      <c r="I67" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="J67" s="5" t="s">
+      <c r="J67" s="6" t="s">
         <v>19</v>
       </c>
       <c r="K67" s="2" t="s">
@@ -4908,13 +4981,13 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B68" s="1" t="s">
+      <c r="A68" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -4929,13 +5002,13 @@
       <c r="G68" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H68" s="6" t="s">
         <v>486</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="J68" s="5" t="s">
+      <c r="J68" s="6" t="s">
         <v>488</v>
       </c>
       <c r="K68" s="2" t="s">
@@ -4943,13 +5016,13 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B69" s="1" t="s">
+      <c r="A69" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -4964,13 +5037,13 @@
       <c r="G69" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H69" s="5" t="s">
+      <c r="H69" s="6" t="s">
         <v>493</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="J69" s="5" t="s">
+      <c r="J69" s="6" t="s">
         <v>495</v>
       </c>
       <c r="K69" s="2" t="s">
@@ -4978,13 +5051,13 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B70" s="1" t="s">
+      <c r="A70" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B70" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -4999,13 +5072,13 @@
       <c r="G70" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="H70" s="6" t="s">
         <v>500</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="J70" s="5" t="s">
+      <c r="J70" s="6" t="s">
         <v>433</v>
       </c>
       <c r="K70" s="2" t="s">
@@ -5013,13 +5086,13 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B71" s="1" t="s">
+      <c r="A71" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -5034,13 +5107,13 @@
       <c r="G71" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H71" s="6" t="s">
         <v>507</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="J71" s="5" t="s">
+      <c r="J71" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K71" s="2" t="s">
@@ -5048,13 +5121,13 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B72" s="1" t="s">
+      <c r="A72" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -5069,13 +5142,13 @@
       <c r="G72" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H72" s="5" t="s">
+      <c r="H72" s="6" t="s">
         <v>513</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="J72" s="5" t="s">
+      <c r="J72" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K72" s="2" t="s">
@@ -5083,13 +5156,13 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B73" s="1" t="s">
+      <c r="A73" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -5104,13 +5177,13 @@
       <c r="G73" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="H73" s="6" t="s">
         <v>520</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="J73" s="5" t="s">
+      <c r="J73" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K73" s="2" t="s">
@@ -5118,13 +5191,13 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B74" s="1" t="s">
+      <c r="A74" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -5139,13 +5212,13 @@
       <c r="G74" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="H74" s="6" t="s">
         <v>295</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="J74" s="5" t="s">
+      <c r="J74" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K74" s="2" t="s">
@@ -5153,13 +5226,13 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B75" s="1" t="s">
+      <c r="A75" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -5174,13 +5247,13 @@
       <c r="G75" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="H75" s="5" t="s">
+      <c r="H75" s="6" t="s">
         <v>531</v>
       </c>
       <c r="I75" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="J75" s="5" t="s">
+      <c r="J75" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K75" s="2" t="s">
@@ -5188,13 +5261,13 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B76" s="1" t="s">
+      <c r="A76" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -5209,13 +5282,13 @@
       <c r="G76" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="H76" s="5" t="s">
+      <c r="H76" s="6" t="s">
         <v>538</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="J76" s="5" t="s">
+      <c r="J76" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K76" s="2" t="s">
@@ -5223,13 +5296,13 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B77" s="1" t="s">
+      <c r="A77" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B77" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -5244,13 +5317,13 @@
       <c r="G77" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="H77" s="5" t="s">
+      <c r="H77" s="6" t="s">
         <v>545</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="J77" s="5" t="s">
+      <c r="J77" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K77" s="2" t="s">
@@ -5258,13 +5331,13 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B78" s="1" t="s">
+      <c r="A78" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B78" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -5279,13 +5352,13 @@
       <c r="G78" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="H78" s="5" t="s">
+      <c r="H78" s="6" t="s">
         <v>552</v>
       </c>
       <c r="I78" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="J78" s="5" t="s">
+      <c r="J78" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K78" s="2" t="s">
@@ -5293,13 +5366,13 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B79" s="1" t="s">
+      <c r="A79" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -5314,13 +5387,13 @@
       <c r="G79" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="H79" s="5" t="s">
+      <c r="H79" s="6" t="s">
         <v>559</v>
       </c>
-      <c r="I79" s="5" t="s">
+      <c r="I79" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="J79" s="5" t="s">
+      <c r="J79" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K79" s="2" t="s">
@@ -5328,13 +5401,13 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B80" s="1" t="s">
+      <c r="A80" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -5349,13 +5422,13 @@
       <c r="G80" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="H80" s="5" t="s">
+      <c r="H80" s="6" t="s">
         <v>566</v>
       </c>
-      <c r="I80" s="5" t="s">
+      <c r="I80" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="J80" s="5" t="s">
+      <c r="J80" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K80" s="2" t="s">
@@ -5363,13 +5436,13 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B81" s="1" t="s">
+      <c r="A81" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -5384,13 +5457,13 @@
       <c r="G81" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H81" s="5" t="s">
+      <c r="H81" s="6" t="s">
         <v>573</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="J81" s="5" t="s">
+      <c r="J81" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K81" s="2" t="s">
@@ -5398,13 +5471,13 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B82" s="1" t="s">
+      <c r="A82" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -5419,13 +5492,13 @@
       <c r="G82" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="H82" s="5" t="s">
+      <c r="H82" s="6" t="s">
         <v>580</v>
       </c>
-      <c r="I82" s="5" t="s">
+      <c r="I82" s="6" t="s">
         <v>581</v>
       </c>
-      <c r="J82" s="5" t="s">
+      <c r="J82" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K82" s="2" t="s">
@@ -5433,13 +5506,13 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B83" s="1" t="s">
+      <c r="A83" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B83" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -5454,13 +5527,13 @@
       <c r="G83" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="H83" s="5" t="s">
+      <c r="H83" s="6" t="s">
         <v>587</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="J83" s="5" t="s">
+      <c r="J83" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K83" s="2" t="s">
@@ -5468,13 +5541,13 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B84" s="1" t="s">
+      <c r="A84" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -5489,13 +5562,13 @@
       <c r="G84" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="H84" s="5" t="s">
+      <c r="H84" s="6" t="s">
         <v>594</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="J84" s="5" t="s">
+      <c r="J84" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K84" s="2" t="s">
@@ -5503,13 +5576,13 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B85" s="1" t="s">
+      <c r="A85" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -5524,13 +5597,13 @@
       <c r="G85" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="H85" s="5" t="s">
+      <c r="H85" s="6" t="s">
         <v>601</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="J85" s="5" t="s">
+      <c r="J85" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K85" s="2" t="s">
@@ -5538,13 +5611,13 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B86" s="1" t="s">
+      <c r="A86" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -5559,13 +5632,13 @@
       <c r="G86" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="H86" s="5" t="s">
+      <c r="H86" s="6" t="s">
         <v>608</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="J86" s="5" t="s">
+      <c r="J86" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K86" s="2" t="s">
@@ -5573,13 +5646,13 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B87" s="1" t="s">
+      <c r="A87" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -5594,13 +5667,13 @@
       <c r="G87" s="2" t="s">
         <v>614</v>
       </c>
-      <c r="H87" s="5" t="s">
+      <c r="H87" s="6" t="s">
         <v>615</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="J87" s="5" t="s">
+      <c r="J87" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K87" s="2" t="s">
@@ -5608,13 +5681,13 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B88" s="1" t="s">
+      <c r="A88" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -5629,13 +5702,13 @@
       <c r="G88" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="H88" s="5" t="s">
+      <c r="H88" s="6" t="s">
         <v>622</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="J88" s="5" t="s">
+      <c r="J88" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K88" s="2" t="s">
@@ -5643,13 +5716,13 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B89" s="1" t="s">
+      <c r="A89" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B89" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -5664,10 +5737,10 @@
       <c r="G89" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="H89" s="5" t="s">
+      <c r="H89" s="6" t="s">
         <v>628</v>
       </c>
-      <c r="J89" s="5" t="s">
+      <c r="J89" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K89" s="2" t="s">
@@ -5675,13 +5748,13 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B90" s="1" t="s">
+      <c r="A90" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -5693,13 +5766,13 @@
       <c r="F90" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="H90" s="5" t="s">
+      <c r="H90" s="6" t="s">
         <v>633</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>634</v>
       </c>
-      <c r="J90" s="5" t="s">
+      <c r="J90" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K90" s="2" t="s">
@@ -5707,13 +5780,13 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B91" s="1" t="s">
+      <c r="A91" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B91" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -5728,13 +5801,13 @@
       <c r="G91" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="H91" s="5" t="s">
+      <c r="H91" s="6" t="s">
         <v>639</v>
       </c>
       <c r="I91" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="J91" s="5" t="s">
+      <c r="J91" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K91" s="2" t="s">
@@ -5742,13 +5815,13 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B92" s="1" t="s">
+      <c r="A92" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B92" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -5763,13 +5836,13 @@
       <c r="G92" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="H92" s="5" t="s">
+      <c r="H92" s="6" t="s">
         <v>646</v>
       </c>
       <c r="I92" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="J92" s="5" t="s">
+      <c r="J92" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K92" s="2" t="s">
@@ -5777,13 +5850,13 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B93" s="1" t="s">
+      <c r="A93" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B93" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -5798,13 +5871,13 @@
       <c r="G93" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="H93" s="5" t="s">
+      <c r="H93" s="6" t="s">
         <v>653</v>
       </c>
       <c r="I93" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="J93" s="5" t="s">
+      <c r="J93" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K93" s="2" t="s">
@@ -5812,13 +5885,13 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B94" s="1" t="s">
+      <c r="A94" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -5833,13 +5906,13 @@
       <c r="G94" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="H94" s="5" t="s">
+      <c r="H94" s="6" t="s">
         <v>659</v>
       </c>
       <c r="I94" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="J94" s="5" t="s">
+      <c r="J94" s="6" t="s">
         <v>218</v>
       </c>
       <c r="K94" s="2" t="s">
@@ -5847,13 +5920,13 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B95" s="1" t="s">
+      <c r="A95" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B95" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -5868,13 +5941,13 @@
       <c r="G95" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="H95" s="5" t="s">
+      <c r="H95" s="6" t="s">
         <v>665</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="J95" s="5" t="s">
+      <c r="J95" s="6" t="s">
         <v>218</v>
       </c>
       <c r="K95" s="2" t="s">
@@ -5882,13 +5955,13 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B96" s="1" t="s">
+      <c r="A96" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -5903,13 +5976,13 @@
       <c r="G96" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="H96" s="5" t="s">
+      <c r="H96" s="6" t="s">
         <v>672</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>673</v>
       </c>
-      <c r="J96" s="5" t="s">
+      <c r="J96" s="6" t="s">
         <v>297</v>
       </c>
       <c r="K96" s="2" t="s">
@@ -5917,13 +5990,13 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B97" s="1" t="s">
+      <c r="A97" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B97" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -5938,13 +6011,13 @@
       <c r="G97" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="H97" s="5" t="s">
+      <c r="H97" s="6" t="s">
         <v>679</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="J97" s="5" t="s">
+      <c r="J97" s="6" t="s">
         <v>681</v>
       </c>
       <c r="K97" s="2" t="s">
@@ -5952,13 +6025,13 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B98" s="1" t="s">
+      <c r="A98" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -5973,13 +6046,13 @@
       <c r="G98" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="H98" s="5" t="s">
+      <c r="H98" s="6" t="s">
         <v>686</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="J98" s="5" t="s">
+      <c r="J98" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K98" s="2" t="s">
@@ -5987,13 +6060,13 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B99" s="1" t="s">
+      <c r="A99" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B99" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -6008,13 +6081,13 @@
       <c r="G99" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="H99" s="5" t="s">
+      <c r="H99" s="6" t="s">
         <v>692</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>693</v>
       </c>
-      <c r="J99" s="5" t="s">
+      <c r="J99" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K99" s="2" t="s">
@@ -6022,13 +6095,13 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B100" s="1" t="s">
+      <c r="A100" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -6043,13 +6116,13 @@
       <c r="G100" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="H100" s="5" t="s">
+      <c r="H100" s="6" t="s">
         <v>699</v>
       </c>
       <c r="I100" s="2" t="s">
         <v>700</v>
       </c>
-      <c r="J100" s="5" t="s">
+      <c r="J100" s="6" t="s">
         <v>165</v>
       </c>
       <c r="K100" s="2" t="s">
@@ -6057,13 +6130,13 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B101" s="1" t="s">
+      <c r="A101" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B101" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -6078,13 +6151,13 @@
       <c r="G101" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="H101" s="5" t="s">
+      <c r="H101" s="6" t="s">
         <v>706</v>
       </c>
       <c r="I101" s="2" t="s">
         <v>707</v>
       </c>
-      <c r="J101" s="5" t="s">
+      <c r="J101" s="6" t="s">
         <v>708</v>
       </c>
       <c r="K101" s="2" t="s">
@@ -6092,13 +6165,13 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B102" s="1" t="s">
+      <c r="A102" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B102" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -6110,27 +6183,27 @@
       <c r="F102" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="H102" s="5" t="s">
+      <c r="H102" s="6" t="s">
         <v>713</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="J102" s="5" t="s">
+      <c r="J102" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K102" s="5" t="s">
+      <c r="K102" s="6" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B103" s="1" t="s">
+      <c r="A103" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B103" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -6142,27 +6215,27 @@
       <c r="F103" s="2" t="s">
         <v>718</v>
       </c>
-      <c r="H103" s="5" t="s">
+      <c r="H103" s="6" t="s">
         <v>719</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="J103" s="5" t="s">
+      <c r="J103" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K103" s="5" t="s">
+      <c r="K103" s="6" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B104" s="1" t="s">
+      <c r="A104" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B104" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="5" t="s">
         <v>482</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -6180,7 +6253,7 @@
       <c r="I104" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="J104" s="5" t="s">
+      <c r="J104" s="6" t="s">
         <v>19</v>
       </c>
       <c r="K104" s="2" t="s">

</xml_diff>

<commit_message>
add reference to framework
</commit_message>
<xml_diff>
--- a/storage/app/repository/ISO27001-2022.fr.xlsx
+++ b/storage/app/repository/ISO27001-2022.fr.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">SMSI</t>
   </si>
   <si>
-    <t xml:space="preserve">10.1</t>
+    <t xml:space="preserve">27001:2022-10.1</t>
   </si>
   <si>
     <t xml:space="preserve">Amélioration continue</t>
@@ -83,7 +83,7 @@
     <t xml:space="preserve">Améliorer continuellement la pertinence, l'adéquation et l'efficacité du système de management de la sécurité de l'information.</t>
   </si>
   <si>
-    <t xml:space="preserve">10.2</t>
+    <t xml:space="preserve">27001:2022-10.2</t>
   </si>
   <si>
     <t xml:space="preserve">Non-conformité et actions correctives</t>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">Mettre en place un plan de gestion des non-conformités et des actions correctives</t>
   </si>
   <si>
-    <t xml:space="preserve">4.x</t>
+    <t xml:space="preserve">27001:2022-4.x</t>
   </si>
   <si>
     <t xml:space="preserve">Compréhension de l'organisation et de son contexte</t>
@@ -128,7 +128,7 @@
     <t xml:space="preserve">Sécurité organisationnelle</t>
   </si>
   <si>
-    <t xml:space="preserve">5.01 </t>
+    <t xml:space="preserve">27001:2022-5.01 </t>
   </si>
   <si>
     <t xml:space="preserve">Politiques de sécurité de l'information</t>
@@ -156,7 +156,7 @@
     <t xml:space="preserve">Définir une politique de sécurité de l'information et des politiques portant sur des thèmes, de les faire approuver par la direction, de les publier, de les communiquer et d'en demander confirmation au personnel et aux parties intéressées concernés, ainsi que de les réviser à intervalles planifiés et si des changements notoires interviennent.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.02 </t>
+    <t xml:space="preserve">27001:2022-5.02 </t>
   </si>
   <si>
     <t xml:space="preserve">Fonctions et responsabilités liées à la sécurité de l'information</t>
@@ -183,7 +183,7 @@
     <t xml:space="preserve">Définir et attribuer toutes les responsabilités en matière de sécurité de l’information.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.03 </t>
+    <t xml:space="preserve">27001:2022-5.03 </t>
   </si>
   <si>
     <t xml:space="preserve">Séparation des tâches</t>
@@ -209,7 +209,7 @@
     <t xml:space="preserve">Séparer les tâches et domaines de responsabilité incompatibles.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.04 </t>
+    <t xml:space="preserve">27001:2022-5.04 </t>
   </si>
   <si>
     <t xml:space="preserve">Responsabilités de la direction</t>
@@ -236,7 +236,7 @@
     <t xml:space="preserve">Publier une communication de la direction sur l'importance de la sécurité de l'information pour l'organisation.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.05 </t>
+    <t xml:space="preserve">27001:2022-5.05 </t>
   </si>
   <si>
     <t xml:space="preserve">Relations avec les autorités</t>
@@ -265,7 +265,7 @@
     <t xml:space="preserve">Des relations appropriées avec les autorités compétentes doivent être entretenues.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.06 </t>
+    <t xml:space="preserve">27001:2022-5.06 </t>
   </si>
   <si>
     <t xml:space="preserve">Relations avec des groupes de travail spécialisés</t>
@@ -294,7 +294,7 @@
     <t xml:space="preserve">Revoir la procédure, mettre à jour l'inventaire et entretenir des relations avec les groupes de spécialistes.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.07 </t>
+    <t xml:space="preserve">27001:2022-5.07 </t>
   </si>
   <si>
     <t xml:space="preserve">Intelligence des menaces</t>
@@ -316,7 +316,7 @@
     <t xml:space="preserve">Recueillir et analyser des informations sur les menaces.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.08 </t>
+    <t xml:space="preserve">27001:2022-5.08 </t>
   </si>
   <si>
     <t xml:space="preserve">Sécurité de l'information dans la gestion de projet</t>
@@ -343,7 +343,7 @@
     <t xml:space="preserve">Intégrer la sécurité de l'information aux activités de gestion de projet de l'organisation.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.09 </t>
+    <t xml:space="preserve">27001:2022-5.09 </t>
   </si>
   <si>
     <t xml:space="preserve">Inventaire des informations et des autres actifs associés</t>
@@ -366,7 +366,7 @@
     <t xml:space="preserve">Elaborer et de tenir à jour un inventaire des informations et des autres actifs associés, y compris leurs propriétaires.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.10 </t>
+    <t xml:space="preserve">27001:2022-5.10 </t>
   </si>
   <si>
     <t xml:space="preserve">Utilisation correcte de l'information et des autres actifs associés</t>
@@ -389,7 +389,7 @@
     <t xml:space="preserve">Identifier, documenter et mettre en oeuvre des règles d'utilisation correcte et des procédures de traitement de l'information et des autres actifs associés.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.11 </t>
+    <t xml:space="preserve">27001:2022-5.11 </t>
   </si>
   <si>
     <t xml:space="preserve">Restitution des actifs</t>
@@ -416,7 +416,7 @@
     <t xml:space="preserve">Le personnel et les autres parties intéressées, au besoin, restituent tous les actifs de l'organisation qui sont en leur possession en cas de modification ou de rupture de leur relation de travail, contrat de travail ou engagement.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.12 </t>
+    <t xml:space="preserve">27001:2022-5.12 </t>
   </si>
   <si>
     <t xml:space="preserve">Classification de l'information</t>
@@ -438,7 +438,7 @@
     <t xml:space="preserve">Classifier l'information conformément aux besoins de l'organisation en termes de sécurité de l'information sur le plan de la confidentialité, de l'intégrité, de la disponibilité et des exigences des parties intéressées.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.13 </t>
+    <t xml:space="preserve">27001:2022-5.13 </t>
   </si>
   <si>
     <t xml:space="preserve">Marquage des informations</t>
@@ -460,7 +460,7 @@
     <t xml:space="preserve">Revoir la procédure de marquage de l'information et son application</t>
   </si>
   <si>
-    <t xml:space="preserve">5.14 </t>
+    <t xml:space="preserve">27001:2022-5.14 </t>
   </si>
   <si>
     <t xml:space="preserve">Transfert de l'information</t>
@@ -483,7 +483,7 @@
     <t xml:space="preserve">Mettre en place des politiques, des procédures et des mesures de transfert formelles pour protéger les transferts d’information transitant par tous types d’équipements de communication.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.15 </t>
+    <t xml:space="preserve">27001:2022-5.15 </t>
   </si>
   <si>
     <t xml:space="preserve">Contrôle d'accès</t>
@@ -506,7 +506,7 @@
     <t xml:space="preserve">Etablir, documenter et revoir la politique de contrôle d'accès</t>
   </si>
   <si>
-    <t xml:space="preserve">5.16 </t>
+    <t xml:space="preserve">27001:2022-5.16 </t>
   </si>
   <si>
     <t xml:space="preserve">Gestion des identités</t>
@@ -525,7 +525,7 @@
     <t xml:space="preserve">Gérer le cycle de vie complet des identités.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.17 </t>
+    <t xml:space="preserve">27001:2022-5.17 </t>
   </si>
   <si>
     <t xml:space="preserve">Informations d'authentification</t>
@@ -543,7 +543,7 @@
     <t xml:space="preserve">Mettre en place un processus de gestion formel de l’attribution des informations secrètes d’authentification.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.18 </t>
+    <t xml:space="preserve">27001:2022-5.18 </t>
   </si>
   <si>
     <t xml:space="preserve">Droits d'accès</t>
@@ -568,7 +568,7 @@
     <t xml:space="preserve">Les droits d'accès à l'information et aux autres actifs associés sont mis en service, révisés, modifiés et supprimés conformément à la politique portant sur le thème de l'organisation et aux règles de contrôle d'accès.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.19 </t>
+    <t xml:space="preserve">27001:2022-5.19 </t>
   </si>
   <si>
     <t xml:space="preserve">Sécurité de l'information dans les relations avec les fournisseurs</t>
@@ -591,7 +591,7 @@
     <t xml:space="preserve">Définir et faire accepter par les fournisseurs des exigences de sécurité de l’information pour limiter les risques résultant de l’accès de ces fournisseurs aux actifs de l’organisation.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.20 </t>
+    <t xml:space="preserve">27001:2022-5.20 </t>
   </si>
   <si>
     <t xml:space="preserve">Prise en compte de la sécurité de l'information dans les accords conclus avec les fournisseurs</t>
@@ -608,7 +608,7 @@
     <t xml:space="preserve">Etablir et convenir avec chaque fournisseur pouvant accéder, traiter, stocker, communiquer ou fournir des composants de l’infrastructure informatique destinés à l’information de l’organisation, des exigences applicables liées à la sécurité de l’information.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.21 </t>
+    <t xml:space="preserve">27001:2022-5.21 </t>
   </si>
   <si>
     <t xml:space="preserve">Management de la sécurité de l'information dans la chaîne d'approvisionnement TIC</t>
@@ -625,7 +625,7 @@
     <t xml:space="preserve">Inclure dans les accords conclus avec les fournisseurs, des exigences sur le traitement des risques liés à la sécurité de l’information associé à la chaîne d’approvisionnement des produits et des services informatiques.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.22 </t>
+    <t xml:space="preserve">27001:2022-5.22 </t>
   </si>
   <si>
     <t xml:space="preserve">Suivi, revue et gestion des changements des services fournisseurs</t>
@@ -647,7 +647,7 @@
     <t xml:space="preserve">Surveiller, vérifier et auditer à intervalles réguliers la prestation des services assurés par les fournisseurs.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.23 </t>
+    <t xml:space="preserve">27001:2022-5.23 </t>
   </si>
   <si>
     <t xml:space="preserve">Sécurité de l'information dans l'utilisation de services en nuage</t>
@@ -670,7 +670,7 @@
     <t xml:space="preserve">Définir et surveiller les processus d'acquisition, d'utilisation, de management et de cessation des services en nuage conformément aux exigences de sécurité de l'information de l'organisation</t>
   </si>
   <si>
-    <t xml:space="preserve">5.24 </t>
+    <t xml:space="preserve">27001:2022-5.24 </t>
   </si>
   <si>
     <t xml:space="preserve">Planification et préparation de la gestion des incidents liés à la sécurité de
@@ -694,7 +694,7 @@
     <t xml:space="preserve">Etablir des responsabilités et des procédures permettant de garantir une réponse rapide, efficace et pertinente en cas d’incident lié à la sécurité de l’information.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.25 </t>
+    <t xml:space="preserve">27001:2022-5.25 </t>
   </si>
   <si>
     <t xml:space="preserve">Appréciation des événements liés à la sécurité de l'information et prise de décision</t>
@@ -717,7 +717,7 @@
     <t xml:space="preserve">Revoir le processus d'appréciation des incidents</t>
   </si>
   <si>
-    <t xml:space="preserve">5.26 </t>
+    <t xml:space="preserve">27001:2022-5.26 </t>
   </si>
   <si>
     <t xml:space="preserve">Réponse aux incidents liés à la sécurité de l'information</t>
@@ -745,7 +745,7 @@
     <t xml:space="preserve">Traiter les incidents liés à la sécurité de l’information conformément aux procédures documentées.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.27 </t>
+    <t xml:space="preserve">27001:2022-5.27 </t>
   </si>
   <si>
     <t xml:space="preserve">Tirer des enseignements des incidents liés à la sécurité de l'information</t>
@@ -768,7 +768,7 @@
     <t xml:space="preserve">Utiliser les connaissances recueillies suite à l’analyse et la résolution d’incidents pour réduire la probabilité ou l’impact d’incidents ultérieurs.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.28 </t>
+    <t xml:space="preserve">27001:2022-5.28 </t>
   </si>
   <si>
     <t xml:space="preserve">Recueil de preuves</t>
@@ -796,7 +796,7 @@
     <t xml:space="preserve">Définir et appliquer des procédures d’identification, de collecte, d’acquisition et de protection de l’information pouvant servir de preuve.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.29 </t>
+    <t xml:space="preserve">27001:2022-5.29 </t>
   </si>
   <si>
     <t xml:space="preserve">Sécurité de l'information durant une perturbation</t>
@@ -820,7 +820,7 @@
     <t xml:space="preserve">Déterminer ses exigences en matière de sécurité de l’information et de continuité de management de la sécurité de l’information dans des situations défavorables, comme lors d’une crise ou d’un sinistre.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.30 </t>
+    <t xml:space="preserve">27001:2022-5.30 </t>
   </si>
   <si>
     <t xml:space="preserve">Préparation des TIC pour la continuité d'activité</t>
@@ -844,7 +844,7 @@
     <t xml:space="preserve">Identifier les objectifs de continuité d'action et les exigences de continuité des TIC. Réaliser des tests de continuité.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.31 </t>
+    <t xml:space="preserve">27001:2022-5.31 </t>
   </si>
   <si>
     <t xml:space="preserve">Identification des exigences légales, statutaires, réglementaires et contractuelles</t>
@@ -866,7 +866,7 @@
     <t xml:space="preserve">Définir explicitement, documenter et mettre à jour toutes les exigences légales, statutaires, réglementaires et contractuelles en vigueur, ainsi que l’approche adoptée par l’organisation pour satisfaire à ces exigences pour chaque système d’information et pour l’organisation elle-même.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.32 </t>
+    <t xml:space="preserve">27001:2022-5.32 </t>
   </si>
   <si>
     <t xml:space="preserve">Droits de propriété intellectuelle</t>
@@ -888,7 +888,7 @@
     <t xml:space="preserve">Mettre en œuvre des procédures appropriées pour garantir la conformité avec les exigences légales, réglementaires et contractuelles relatives à la propriété intellectuelle et à l’usage des licences de logiciels propriétaires.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.33 </t>
+    <t xml:space="preserve">27001:2022-5.33 </t>
   </si>
   <si>
     <t xml:space="preserve">Protection des enregistrements</t>
@@ -914,7 +914,7 @@
     <t xml:space="preserve">Protéger les enregistrements de la perte, de la destruction, de la falsification, des accès non autorisés et des diffusions non autorisées, conformément aux exigences légales, réglementaires, contractuelles et aux exigences métier.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.34 </t>
+    <t xml:space="preserve">27001:2022-5.34 </t>
   </si>
   <si>
     <t xml:space="preserve">Vie privée et protection des DCP</t>
@@ -936,7 +936,7 @@
     <t xml:space="preserve">Garantir la protection de la vie privée et la protection des données à caractère personnel telles que l’exigent la législation ou les réglementations applicables, et les clauses contractuelles le cas échéant.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.35 </t>
+    <t xml:space="preserve">27001:2022-5.35 </t>
   </si>
   <si>
     <t xml:space="preserve">Revue indépendante de la sécurité de l'information</t>
@@ -959,7 +959,7 @@
     <t xml:space="preserve">Effectuer une revue indépendante de l’approche retenue par l’organisme pour gérer et mettre en œuvre la sécurité de l’information (à savoir le suivi des objectifs de sécurité, les mesures, les politiques, les procédures et les processus relatifs à la sécurité de l’information) et mettre en place un plan de suivi de la revue.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.36 </t>
+    <t xml:space="preserve">27001:2022-5.36 </t>
   </si>
   <si>
     <t xml:space="preserve">Conformité aux politiques et normes de sécurité de l'information</t>
@@ -981,7 +981,7 @@
     <t xml:space="preserve">Examiner les systèmes d’information quant à leur conformité avec les politiques et les normes de sécurité de l’information de l’organisation.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.37 </t>
+    <t xml:space="preserve">27001:2022-5.37 </t>
   </si>
   <si>
     <t xml:space="preserve">Procédures d'exploitation documentées</t>
@@ -1008,7 +1008,7 @@
     <t xml:space="preserve">Documenter et mettre à disposition des utilisateurs concernés les procédures d’exploitation.</t>
   </si>
   <si>
-    <t xml:space="preserve">5.x</t>
+    <t xml:space="preserve">27001:2022-5.x</t>
   </si>
   <si>
     <t xml:space="preserve">Leadership</t>
@@ -1039,7 +1039,7 @@
     <t xml:space="preserve">Sécurité des personnes</t>
   </si>
   <si>
-    <t xml:space="preserve">6.01 </t>
+    <t xml:space="preserve">27001:2022-6.01 </t>
   </si>
   <si>
     <t xml:space="preserve">Présélection</t>
@@ -1066,7 +1066,7 @@
     <t xml:space="preserve">Mettre à jour la procédure et effectuer des vérifications sur tous les candidats à l’embauche.</t>
   </si>
   <si>
-    <t xml:space="preserve">6.02 </t>
+    <t xml:space="preserve">27001:2022-6.02 </t>
   </si>
   <si>
     <t xml:space="preserve">Conditions générales d'embauche</t>
@@ -1090,7 +1090,7 @@
     <t xml:space="preserve">Définir les responsabilités et celles de l’organisation en matière de sécurité de l’information dans les accords contractuels entre les salariés et les sous-traitants.</t>
   </si>
   <si>
-    <t xml:space="preserve">6.03 </t>
+    <t xml:space="preserve">27001:2022-6.03 </t>
   </si>
   <si>
     <t xml:space="preserve">Sensibilisation, apprentissage et formation à la sécurité de l'information</t>
@@ -1117,7 +1117,7 @@
     <t xml:space="preserve">Sensibilier le personnel de l'organisation et les parties intéressées  à la sécurité de l'information, leur communiquer un apprentissage et des formations à la sécurité de l'information adaptés, et leur transmettre régulièrement les mises à jour des politiques et procédures de l'organisation s'appliquant à leur fonction.</t>
   </si>
   <si>
-    <t xml:space="preserve">6.04 </t>
+    <t xml:space="preserve">27001:2022-6.04 </t>
   </si>
   <si>
     <t xml:space="preserve">Processus disciplinaire</t>
@@ -1145,7 +1145,7 @@
     <t xml:space="preserve">Formaliser et communiquer un processus disciplinaire permettant de prendre des mesures à l'encontre du personnel et des autres parties intéressées qui ont commis une violation de la politique de sécurité de l'information.</t>
   </si>
   <si>
-    <t xml:space="preserve">6.05 </t>
+    <t xml:space="preserve">27001:2022-6.05 </t>
   </si>
   <si>
     <t xml:space="preserve">Responsabilités consécutivement à la fin ou à la modification du contrat de tr</t>
@@ -1172,7 +1172,7 @@
     <t xml:space="preserve">Définir les responsabilités et les missions liées à la sécurité de l’information qui restent valables à l’issue de la rupture, du terme ou de la modification du contrat de travail.</t>
   </si>
   <si>
-    <t xml:space="preserve">6.06 </t>
+    <t xml:space="preserve">27001:2022-6.06 </t>
   </si>
   <si>
     <t xml:space="preserve">Engagements de confidentialité ou de non-divulgation</t>
@@ -1194,7 +1194,7 @@
     <t xml:space="preserve">Identifier, vérifier et documenter les exigences en matière d’engagements de confidentialité ou de non-divulgation.</t>
   </si>
   <si>
-    <t xml:space="preserve">6.07 </t>
+    <t xml:space="preserve">27001:2022-6.07 </t>
   </si>
   <si>
     <t xml:space="preserve">Travail à distance</t>
@@ -1216,7 +1216,7 @@
     <t xml:space="preserve">Définir et mettre en oeuvre une politique et des mesures de sécurité complémentaires pour protéger les informations consultées, traitées ou stockées sur des sites de télétravail.</t>
   </si>
   <si>
-    <t xml:space="preserve">6.08 </t>
+    <t xml:space="preserve">27001:2022-6.08 </t>
   </si>
   <si>
     <t xml:space="preserve">Signalement des événements liés à la sécurité de l'information</t>
@@ -1238,7 +1238,7 @@
     <t xml:space="preserve">Signaler les événements liés à la sécurité de l’information dans les meilleurs délais par les voies hiérarchiques appropriées.</t>
   </si>
   <si>
-    <t xml:space="preserve">6.x</t>
+    <t xml:space="preserve">27001:2022-6.x</t>
   </si>
   <si>
     <t xml:space="preserve">Planification</t>
@@ -1269,7 +1269,7 @@
     <t xml:space="preserve">Sécurité physique</t>
   </si>
   <si>
-    <t xml:space="preserve">7.01 </t>
+    <t xml:space="preserve">27001:2022-7.01 </t>
   </si>
   <si>
     <t xml:space="preserve">Périmètre de sécurité physique</t>
@@ -1291,7 +1291,7 @@
     <t xml:space="preserve">Définir des périmètres de sécurité pour protéger les zones contenant l’information sensible ou critique et les moyens de traitement de l’information.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.02 </t>
+    <t xml:space="preserve">27001:2022-7.02 </t>
   </si>
   <si>
     <t xml:space="preserve">Contrôles physiques des accès</t>
@@ -1314,7 +1314,7 @@
     <t xml:space="preserve">Mettre en place des contrôles adéquats à l’entrée des zones sécurisées pour s’assurer que seul le personnel autorisé est admis.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.03 </t>
+    <t xml:space="preserve">27001:2022-7.03 </t>
   </si>
   <si>
     <t xml:space="preserve">Sécurisation des bureaux, des salles et des équipements</t>
@@ -1337,7 +1337,7 @@
     <t xml:space="preserve">Concevoir et appliquer des mesures de sécurité physique aux bureaux, aux salles et aux équipements.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.04 </t>
+    <t xml:space="preserve">27001:2022-7.04 </t>
   </si>
   <si>
     <t xml:space="preserve">Surveillance de la sécurité physique</t>
@@ -1360,7 +1360,7 @@
     <t xml:space="preserve">Identifier les locaux concernés, identifier les mesures à mettre en place et surveiller en continu l'accès physique non autorisé</t>
   </si>
   <si>
-    <t xml:space="preserve">7.05 </t>
+    <t xml:space="preserve">27001:2022-7.05 </t>
   </si>
   <si>
     <t xml:space="preserve">Protection contre les menaces physiques et environnementales</t>
@@ -1380,7 +1380,7 @@
     <t xml:space="preserve">Concevoir et appliquer des mesures de protection physique contre les désastres naturels, les attaques malveillantes ou les accidents.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.06 </t>
+    <t xml:space="preserve">27001:2022-7.06 </t>
   </si>
   <si>
     <t xml:space="preserve">Travail dans les zones sécurisées</t>
@@ -1400,7 +1400,7 @@
     <t xml:space="preserve">Concevoir et appliquer des procédures pour le travail dans les zones sécurisées.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.07 </t>
+    <t xml:space="preserve">27001:2022-7.07 </t>
   </si>
   <si>
     <t xml:space="preserve">Bureau propre et écran vide</t>
@@ -1423,7 +1423,7 @@
 - Sensibiliser les utilisateurs au respect de la politique du bureau propre et de l’écran verrouillé</t>
   </si>
   <si>
-    <t xml:space="preserve">7.08 </t>
+    <t xml:space="preserve">27001:2022-7.08 </t>
   </si>
   <si>
     <t xml:space="preserve">Emplacement et protection du matériel</t>
@@ -1445,7 +1445,7 @@
     <t xml:space="preserve">Protéger les matériels contre les risques liés à des menaces et des dangers environnementaux et les possibilités d’accès non autorisé.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.09 </t>
+    <t xml:space="preserve">27001:2022-7.09 </t>
   </si>
   <si>
     <t xml:space="preserve">Sécurité des actifs hors des locaux</t>
@@ -1469,7 +1469,7 @@
     <t xml:space="preserve">Appliquer des mesures de sécurité aux matériels utilisés hors des locaux de l’organisation en tenant compte des différents risques associés au travail hors site.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.10 </t>
+    <t xml:space="preserve">27001:2022-7.10 </t>
   </si>
   <si>
     <t xml:space="preserve">Supports de stockage</t>
@@ -1494,7 +1494,7 @@
     <t xml:space="preserve">Gérer les supports de stockage tout au long de leur cycle de vie d'acquisition, d'utilisation, de transport et de mise au rebut conformément au plan de classification et aux exigences de manipulation de l'organisation.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.11 </t>
+    <t xml:space="preserve">27001:2022-7.11 </t>
   </si>
   <si>
     <t xml:space="preserve">Services généraux</t>
@@ -1516,7 +1516,7 @@
     <t xml:space="preserve">Protéger les matériels des coupures de courant et autres perturbations dues à une défaillance des services généraux.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.12 </t>
+    <t xml:space="preserve">27001:2022-7.12 </t>
   </si>
   <si>
     <t xml:space="preserve">Sécurité du câblage</t>
@@ -1538,7 +1538,7 @@
     <t xml:space="preserve">Protéger les câbles électriques, transportant des données ou supportant les services d'information contre toute interception, interférence ou tout dommage.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.13 </t>
+    <t xml:space="preserve">27001:2022-7.13 </t>
   </si>
   <si>
     <t xml:space="preserve">Maintenance du matériel</t>
@@ -1561,7 +1561,7 @@
     <t xml:space="preserve">Entretenir correctement les matériels pour garantir leur disponibilité permanente et leur intégrité.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.14 </t>
+    <t xml:space="preserve">27001:2022-7.14 </t>
   </si>
   <si>
     <t xml:space="preserve">Mise au rebut ou recyclage sécurisé(e) du matériel</t>
@@ -1584,7 +1584,7 @@
     <t xml:space="preserve">S’assurer que toute donnée sensible a bien été supprimée et que tout logiciel sous licence a bien été désinstallé ou écrasé de façon sécurisée  du matériel contenant des données sensibles avant leur mise au rebut ou leur réutilisation.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.2</t>
+    <t xml:space="preserve">27001:2022-7.2</t>
   </si>
   <si>
     <t xml:space="preserve">Compétences</t>
@@ -1603,7 +1603,7 @@
     <t xml:space="preserve">Disposer des ressources nécessaires ayant les compétences requises pour la gestion du SMSI.</t>
   </si>
   <si>
-    <t xml:space="preserve">7.x</t>
+    <t xml:space="preserve">27001:2022-7.x</t>
   </si>
   <si>
     <t xml:space="preserve">Support</t>
@@ -1631,7 +1631,7 @@
     <t xml:space="preserve">Sécurité technique</t>
   </si>
   <si>
-    <t xml:space="preserve">8.01 </t>
+    <t xml:space="preserve">27001:2022-8.01 </t>
   </si>
   <si>
     <t xml:space="preserve">Terminaux utilisateurs</t>
@@ -1656,7 +1656,7 @@
     <t xml:space="preserve">Protéger toute information stockée ou traitée sur un terminal utilisateur final ou accessible via ce type d'appareil.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.02 </t>
+    <t xml:space="preserve">27001:2022-8.02 </t>
   </si>
   <si>
     <t xml:space="preserve">Privilèges d'accès</t>
@@ -1680,7 +1680,7 @@
     <t xml:space="preserve">Restreindre et contrôler l’allocation et l’utilisation des droits d’accès à privilèges</t>
   </si>
   <si>
-    <t xml:space="preserve">8.03 </t>
+    <t xml:space="preserve">27001:2022-8.03 </t>
   </si>
   <si>
     <t xml:space="preserve">Restriction d'accès à l'information</t>
@@ -1704,7 +1704,7 @@
     <t xml:space="preserve">Revoir les restrictions d'accès à l'information et leur application</t>
   </si>
   <si>
-    <t xml:space="preserve">8.04 </t>
+    <t xml:space="preserve">27001:2022-8.04 </t>
   </si>
   <si>
     <t xml:space="preserve">Accès au code source</t>
@@ -1726,7 +1726,7 @@
     <t xml:space="preserve">Restreindre l’accès au code source des programmes.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.05 </t>
+    <t xml:space="preserve">27001:2022-8.05 </t>
   </si>
   <si>
     <t xml:space="preserve">Authentification sécurisée</t>
@@ -1745,7 +1745,7 @@
     <t xml:space="preserve">Lorsque la politique de contrôle d’accès l’exige, contrôler par une procédure de connexion sécurisée l'accès aux systèmes et aux applications.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.06 </t>
+    <t xml:space="preserve">27001:2022-8.06 </t>
   </si>
   <si>
     <t xml:space="preserve">Dimensionnement</t>
@@ -1768,7 +1768,7 @@
     <t xml:space="preserve">Surveiller et ajuster l’utilisation des ressources et effectuer des projections sur les dimensionnements futurs pour garantir les performances exigées du système.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.07 </t>
+    <t xml:space="preserve">27001:2022-8.07 </t>
   </si>
   <si>
     <t xml:space="preserve">Protection contre les programmes malveillants</t>
@@ -1780,7 +1780,7 @@
     <t xml:space="preserve">#Préventive #Détective #Corrective #Confidentialité #Intégrité #Disponibilité #Protéger #Détecter #Sécurité_système_et_réseau #Protection_des_informations #Protection #Défense</t>
   </si>
   <si>
-    <t xml:space="preserve">8.08 </t>
+    <t xml:space="preserve">27001:2022-8.08 </t>
   </si>
   <si>
     <t xml:space="preserve">Gestion des vulnérabilités techniques</t>
@@ -1803,7 +1803,7 @@
     <t xml:space="preserve">Obtenir des informations sur les vulnérabilités techniques des systèmes d'information, évaluer l'exposition de l'organisation à ces vulnérabilités et prendre les mesures appropriées.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.09 </t>
+    <t xml:space="preserve">27001:2022-8.09 </t>
   </si>
   <si>
     <t xml:space="preserve">Gestion de la configuration</t>
@@ -1826,7 +1826,7 @@
     <t xml:space="preserve">Vérifier le matériel, les logiciels, les services et les réseaux afin de s'assurer qu'ils fonctionnent correctement avec les paramètres de sécurité requis, et que la configuration n’est pas altérée par des changements non autorisés ou incorrects.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.10 </t>
+    <t xml:space="preserve">27001:2022-8.10 </t>
   </si>
   <si>
     <t xml:space="preserve">Suppression d'information</t>
@@ -1849,7 +1849,7 @@
     <t xml:space="preserve">Supprimer l'information stockée dans les systèmes d'information et les dispositifs lorsqu'elle n'est plus utile.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.11 </t>
+    <t xml:space="preserve">27001:2022-8.11 </t>
   </si>
   <si>
     <t xml:space="preserve">Masquage des données</t>
@@ -1872,7 +1872,7 @@
     <t xml:space="preserve">Utiliser le masquage des données conformément à la politique de l'organisation portant sur le thème du contrôle d'accès et aux exigences métier, tout en prenant en compte les exigences d'ordre légal.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.12 </t>
+    <t xml:space="preserve">27001:2022-8.12 </t>
   </si>
   <si>
     <t xml:space="preserve">Prévention de la fuite de données</t>
@@ -1897,7 +1897,7 @@
     <t xml:space="preserve">Appliquer des mesures de prévention de la fuite de données aux systèmes, réseaux et terminaux qui traitent, stockent ou transmettent de l'information sensible.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.13 </t>
+    <t xml:space="preserve">27001:2022-8.13 </t>
   </si>
   <si>
     <t xml:space="preserve">Sauvegarde des informations</t>
@@ -1922,7 +1922,7 @@
     <t xml:space="preserve">Conserver des copies de sauvegarde de l'information, des logiciels et des systèmes et de les tester régulièrement à l'aide de la politique définie sur le thème de la sauvegarde.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.14 </t>
+    <t xml:space="preserve">27001:2022-8.14 </t>
   </si>
   <si>
     <t xml:space="preserve">Redondance des moyens de traitement de l'information</t>
@@ -1945,7 +1945,7 @@
     <t xml:space="preserve">Mettre en œuvre des moyens de traitement de l’information avec suffisamment de redondances pour répondre aux exigences de disponibilité.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.15 </t>
+    <t xml:space="preserve">27001:2022-8.15 </t>
   </si>
   <si>
     <t xml:space="preserve">Journalisation</t>
@@ -1970,7 +1970,7 @@
     <t xml:space="preserve">Créer, protéger, stocker et dnalyser des journaux enregistrant les activités, exceptions, pannes et autres événements pertinents.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.16 </t>
+    <t xml:space="preserve">27001:2022-8.16 </t>
   </si>
   <si>
     <t xml:space="preserve">Activités de surveillance</t>
@@ -1993,7 +1993,7 @@
     <t xml:space="preserve">Surveiller les réseaux, systèmes et applications pour détecter tout comportement anormal et de prendre les mesures appropriées pour évaluer les incidents liés à la sécurité de l'information potentiels.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.17 </t>
+    <t xml:space="preserve">27001:2022-8.17 </t>
   </si>
   <si>
     <t xml:space="preserve">Synchronisation des horloges</t>
@@ -2017,7 +2017,7 @@
     <t xml:space="preserve">Synchronisées sur une source de référence temporelle unique les horloges de l’ensemble des systèmes de traitement de l’information concernés d’une organisation ou d’un domaine de sécurité.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.18 </t>
+    <t xml:space="preserve">27001:2022-8.18 </t>
   </si>
   <si>
     <t xml:space="preserve">Utilisation de programmes utilitaires à privilèges</t>
@@ -2039,7 +2039,7 @@
     <t xml:space="preserve">Faire l'inventaire des programmes utilitaires permettant de contourner les mesures de sécurité d’un système ou d’une application, limiter et étroitement contrôler leur utilisation.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.19 </t>
+    <t xml:space="preserve">27001:2022-8.19 </t>
   </si>
   <si>
     <t xml:space="preserve">Installation de logiciels sur des systèmes en exploitation</t>
@@ -2061,7 +2061,7 @@
     <t xml:space="preserve">Mettre en œuvre des procédures sont mises en œuvre pour contrôler l’installation de logiciels dans les systèmes opérationnels.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.20 </t>
+    <t xml:space="preserve">27001:2022-8.20 </t>
   </si>
   <si>
     <t xml:space="preserve">Mesures liées aux réseaux</t>
@@ -2084,7 +2084,7 @@
     <t xml:space="preserve">Gérer et contrôler les réseaux pour protéger l’information contenue dans les systèmes et les applications.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.21 </t>
+    <t xml:space="preserve">27001:2022-8.21 </t>
   </si>
   <si>
     <t xml:space="preserve">Sécurité des services en réseau</t>
@@ -2106,7 +2106,7 @@
     <t xml:space="preserve">Pour tous les services de réseau, identifier et intégrer dans les accords de services de réseau, les mécanismes de sécurité, les niveaux de service et les exigences de gestion.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.22 </t>
+    <t xml:space="preserve">27001:2022-8.22 </t>
   </si>
   <si>
     <t xml:space="preserve">Filtrage Internet</t>
@@ -2125,7 +2125,7 @@
     <t xml:space="preserve">Gérer l'accès aux sites Web externes pour réduire l'exposition à tout contenu malveillant.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.23 </t>
+    <t xml:space="preserve">27001:2022-8.23 </t>
   </si>
   <si>
     <t xml:space="preserve">Cloisonnement des réseaux</t>
@@ -2144,7 +2144,7 @@
     <t xml:space="preserve">Cloisonner sur les réseaux les groupes de services d’information, d’utilisateurs et de systèmes d’information.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.24 </t>
+    <t xml:space="preserve">27001:2022-8.24 </t>
   </si>
   <si>
     <t xml:space="preserve">Utilisation de la cryptographie</t>
@@ -2164,7 +2164,7 @@
     <t xml:space="preserve">Définir et de mettre en oeuvre des règles relatives à l'utilisation de la cryptographie, notamment la gestion des clés cryptographiques.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.25 </t>
+    <t xml:space="preserve">27001:2022-8.25 </t>
   </si>
   <si>
     <t xml:space="preserve">Cycle de vie de développement sécurisé</t>
@@ -2187,7 +2187,7 @@
     <t xml:space="preserve">Etablir et appliquer des règles de développement des logiciels et des systèmes aux développements de l’organisation.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.26 </t>
+    <t xml:space="preserve">27001:2022-8.26 </t>
   </si>
   <si>
     <t xml:space="preserve">Exigences de sécurité des applications</t>
@@ -2209,7 +2209,7 @@
     <t xml:space="preserve">Protéger contre les activités frauduleuses, les différents contractuels, ainsi que la divulgation et la modification non autorisées les informations liées aux services d’application transmises sur les réseaux publics.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.27 </t>
+    <t xml:space="preserve">27001:2022-8.27 </t>
   </si>
   <si>
     <t xml:space="preserve">Principes d'ingénierie et d'architecture système sécurisée</t>
@@ -2228,7 +2228,7 @@
     <t xml:space="preserve">Etablir et documenter des principes d’ingénierie de la sécurité des systèmes, les tenir à jour et les appliquer à tous les travaux de mise en œuvre des systèmes d’information.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.28 </t>
+    <t xml:space="preserve">27001:2022-8.28 </t>
   </si>
   <si>
     <t xml:space="preserve">Codage sécurisé</t>
@@ -2247,7 +2247,7 @@
     <t xml:space="preserve">Appliquer des principes de codage sécurisé au développement de logiciels.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.29 </t>
+    <t xml:space="preserve">27001:2022-8.29 </t>
   </si>
   <si>
     <t xml:space="preserve">Tests de sécurité dans le développement et l'acceptation</t>
@@ -2270,7 +2270,7 @@
     <t xml:space="preserve">Réaliser des tests de fonctionnalité de la sécurité pendant le développement.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.30 </t>
+    <t xml:space="preserve">27001:2022-8.30 </t>
   </si>
   <si>
     <t xml:space="preserve">Développement externalisé</t>
@@ -2297,7 +2297,7 @@
     <t xml:space="preserve">Superviser et contrôler l’activité de développement du système externalisée.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.31 </t>
+    <t xml:space="preserve">27001:2022-8.31 </t>
   </si>
   <si>
     <t xml:space="preserve">Séparation des environnements de développement, de test et de production</t>
@@ -2317,7 +2317,7 @@
     <t xml:space="preserve">Séparer les environnements de développement, de test et d’exploitation pour réduire les risques d’accès ou de changements non autorisés dans l’environnement en exploitation.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.32 </t>
+    <t xml:space="preserve">27001:2022-8.32 </t>
   </si>
   <si>
     <t xml:space="preserve">Gestion des changements</t>
@@ -2336,7 +2336,7 @@
     <t xml:space="preserve">Contrôler les changements des systèmes dans le cadre du cycle de développement par le biais de procédures formelles.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.33 </t>
+    <t xml:space="preserve">27001:2022-8.33 </t>
   </si>
   <si>
     <t xml:space="preserve">Informations relatives aux tests</t>
@@ -2358,7 +2358,7 @@
     <t xml:space="preserve">Sélectionner avec soin, protéger et contrôler les données de test.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.34 </t>
+    <t xml:space="preserve">27001:2022-8.34 </t>
   </si>
   <si>
     <t xml:space="preserve">Protection des systèmes d'information en cours d'audit et de test</t>
@@ -2386,7 +2386,7 @@
     <t xml:space="preserve">Prévoir avec soin et valider les exigences et activités d’audit impliquant des vérifications sur des systèmes en exploitation afin de réduire au minimum les perturbations subies par les processus métier.</t>
   </si>
   <si>
-    <t xml:space="preserve">8.x</t>
+    <t xml:space="preserve">27001:2022-8.x</t>
   </si>
   <si>
     <t xml:space="preserve">Fonctionnement</t>
@@ -2408,7 +2408,7 @@
 Mettre en œuvre le plan de traitement des risques de sécurité de l’information.</t>
   </si>
   <si>
-    <t xml:space="preserve">9.2</t>
+    <t xml:space="preserve">27001:2022-9.2</t>
   </si>
   <si>
     <t xml:space="preserve">Audit Interne</t>
@@ -2430,7 +2430,7 @@
 Suivre les recommandations d'audit dans un plan d'action</t>
   </si>
   <si>
-    <t xml:space="preserve">9.3</t>
+    <t xml:space="preserve">27001:2022-9.3</t>
   </si>
   <si>
     <t xml:space="preserve">Revue de Direction</t>
@@ -2679,19 +2679,19 @@
   <dimension ref="A1:K104"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="14.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="18.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="48.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="63.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="4" width="50"/>
@@ -2736,7 +2736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="377.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
         <v>11</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="364.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
         <v>11</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
         <v>11</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
         <v>11</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
         <v>11</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
         <v>11</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
         <v>11</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="391" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
         <v>11</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="337.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
         <v>11</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
         <v>11</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
         <v>11</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
         <v>11</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
         <v>11</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
         <v>11</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
         <v>11</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
         <v>11</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
         <v>11</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
         <v>11</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="417.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
         <v>11</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
         <v>11</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="485.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
         <v>11</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
         <v>11</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
         <v>11</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="364.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
         <v>11</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
         <v>11</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
         <v>11</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
         <v>11</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="444.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
         <v>11</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
         <v>11</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
         <v>11</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
         <v>11</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
         <v>11</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
         <v>11</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
         <v>11</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
         <v>11</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
         <v>11</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
         <v>11</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
         <v>11</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
         <v>11</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="377.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
         <v>11</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
         <v>11</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
         <v>11</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="766.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
         <v>11</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
         <v>11</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
         <v>11</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
         <v>11</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
         <v>11</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
         <v>11</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
         <v>11</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
         <v>11</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
         <v>11</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
         <v>11</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="9" t="s">
         <v>11</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9" t="s">
         <v>11</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="9" t="s">
         <v>11</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
         <v>11</v>
       </c>
@@ -5277,7 +5277,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
         <v>11</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
         <v>11</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
         <v>11</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="9" t="s">
         <v>11</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
         <v>11</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
         <v>11</v>
       </c>
@@ -5487,7 +5487,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
         <v>11</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="9" t="s">
         <v>11</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="9" t="s">
         <v>11</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
         <v>11</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
         <v>11</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
         <v>11</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
         <v>11</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="350.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="9" t="s">
         <v>11</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="9" t="s">
         <v>11</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="9" t="s">
         <v>11</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="9" t="s">
         <v>11</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="9" t="s">
         <v>11</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="9" t="s">
         <v>11</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="9" t="s">
         <v>11</v>
       </c>
@@ -5977,7 +5977,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
         <v>11</v>
       </c>
@@ -6012,7 +6012,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="9" t="s">
         <v>11</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="9" t="s">
         <v>11</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="9" t="s">
         <v>11</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="9" t="s">
         <v>11</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="9" t="s">
         <v>11</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="9" t="s">
         <v>11</v>
       </c>
@@ -6222,7 +6222,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="9" t="s">
         <v>11</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="9" t="s">
         <v>11</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="9" t="s">
         <v>11</v>
       </c>

</xml_diff>